<commit_message>
221225 판다스 study 2 openpyxl, workbook 활용 1차 완성 완료
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -592,7 +592,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (2).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (10).xlsx</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (3).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (11).xlsx</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -846,7 +846,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (4).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (12).xlsx</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (5).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (13).xlsx</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1100,7 +1100,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (6).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (14).xlsx</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1227,7 +1227,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (7).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (15).xlsx</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1354,7 +1354,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (8).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (16).xlsx</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1481,7 +1481,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터 - 복사본 (9).xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (17).xlsx</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1608,7 +1608,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5.북부여성발전센터.xlsx</t>
+          <t>5.북부여성발전센터 - 복사본 (18).xlsx</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1729,6 +1729,2673 @@
         <v>24212016310</v>
       </c>
       <c r="AG10" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (19).xlsx</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L11" t="n">
+        <v>4</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>135</v>
+      </c>
+      <c r="T11" t="n">
+        <v>36</v>
+      </c>
+      <c r="U11" t="n">
+        <v>255</v>
+      </c>
+      <c r="V11" t="n">
+        <v>800</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X11" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC11" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF11" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (2).xlsx</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P12" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>135</v>
+      </c>
+      <c r="T12" t="n">
+        <v>36</v>
+      </c>
+      <c r="U12" t="n">
+        <v>255</v>
+      </c>
+      <c r="V12" t="n">
+        <v>800</v>
+      </c>
+      <c r="W12" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X12" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC12" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF12" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (20).xlsx</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P13" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>135</v>
+      </c>
+      <c r="T13" t="n">
+        <v>36</v>
+      </c>
+      <c r="U13" t="n">
+        <v>255</v>
+      </c>
+      <c r="V13" t="n">
+        <v>800</v>
+      </c>
+      <c r="W13" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X13" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC13" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF13" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (21).xlsx</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P14" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>135</v>
+      </c>
+      <c r="T14" t="n">
+        <v>36</v>
+      </c>
+      <c r="U14" t="n">
+        <v>255</v>
+      </c>
+      <c r="V14" t="n">
+        <v>800</v>
+      </c>
+      <c r="W14" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X14" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC14" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF14" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (22).xlsx</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L15" t="n">
+        <v>4</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P15" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>135</v>
+      </c>
+      <c r="T15" t="n">
+        <v>36</v>
+      </c>
+      <c r="U15" t="n">
+        <v>255</v>
+      </c>
+      <c r="V15" t="n">
+        <v>800</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X15" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC15" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF15" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (23).xlsx</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L16" t="n">
+        <v>4</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P16" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>135</v>
+      </c>
+      <c r="T16" t="n">
+        <v>36</v>
+      </c>
+      <c r="U16" t="n">
+        <v>255</v>
+      </c>
+      <c r="V16" t="n">
+        <v>800</v>
+      </c>
+      <c r="W16" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X16" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF16" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (24).xlsx</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L17" t="n">
+        <v>4</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P17" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>135</v>
+      </c>
+      <c r="T17" t="n">
+        <v>36</v>
+      </c>
+      <c r="U17" t="n">
+        <v>255</v>
+      </c>
+      <c r="V17" t="n">
+        <v>800</v>
+      </c>
+      <c r="W17" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X17" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC17" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF17" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (25).xlsx</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L18" t="n">
+        <v>4</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P18" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>135</v>
+      </c>
+      <c r="T18" t="n">
+        <v>36</v>
+      </c>
+      <c r="U18" t="n">
+        <v>255</v>
+      </c>
+      <c r="V18" t="n">
+        <v>800</v>
+      </c>
+      <c r="W18" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X18" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC18" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF18" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (26).xlsx</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L19" t="n">
+        <v>4</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P19" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>135</v>
+      </c>
+      <c r="T19" t="n">
+        <v>36</v>
+      </c>
+      <c r="U19" t="n">
+        <v>255</v>
+      </c>
+      <c r="V19" t="n">
+        <v>800</v>
+      </c>
+      <c r="W19" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X19" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC19" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF19" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (27).xlsx</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L20" t="n">
+        <v>4</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P20" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>135</v>
+      </c>
+      <c r="T20" t="n">
+        <v>36</v>
+      </c>
+      <c r="U20" t="n">
+        <v>255</v>
+      </c>
+      <c r="V20" t="n">
+        <v>800</v>
+      </c>
+      <c r="W20" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC20" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF20" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (28).xlsx</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L21" t="n">
+        <v>4</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P21" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>135</v>
+      </c>
+      <c r="T21" t="n">
+        <v>36</v>
+      </c>
+      <c r="U21" t="n">
+        <v>255</v>
+      </c>
+      <c r="V21" t="n">
+        <v>800</v>
+      </c>
+      <c r="W21" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X21" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC21" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF21" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (29).xlsx</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L22" t="n">
+        <v>4</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P22" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>135</v>
+      </c>
+      <c r="T22" t="n">
+        <v>36</v>
+      </c>
+      <c r="U22" t="n">
+        <v>255</v>
+      </c>
+      <c r="V22" t="n">
+        <v>800</v>
+      </c>
+      <c r="W22" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X22" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC22" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF22" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (3).xlsx</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L23" t="n">
+        <v>4</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P23" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>135</v>
+      </c>
+      <c r="T23" t="n">
+        <v>36</v>
+      </c>
+      <c r="U23" t="n">
+        <v>255</v>
+      </c>
+      <c r="V23" t="n">
+        <v>800</v>
+      </c>
+      <c r="W23" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X23" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC23" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF23" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (4).xlsx</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L24" t="n">
+        <v>4</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P24" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>135</v>
+      </c>
+      <c r="T24" t="n">
+        <v>36</v>
+      </c>
+      <c r="U24" t="n">
+        <v>255</v>
+      </c>
+      <c r="V24" t="n">
+        <v>800</v>
+      </c>
+      <c r="W24" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X24" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC24" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF24" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (5).xlsx</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L25" t="n">
+        <v>4</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O25" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P25" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>135</v>
+      </c>
+      <c r="T25" t="n">
+        <v>36</v>
+      </c>
+      <c r="U25" t="n">
+        <v>255</v>
+      </c>
+      <c r="V25" t="n">
+        <v>800</v>
+      </c>
+      <c r="W25" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X25" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC25" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE25" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF25" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (6).xlsx</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L26" t="n">
+        <v>4</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P26" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>135</v>
+      </c>
+      <c r="T26" t="n">
+        <v>36</v>
+      </c>
+      <c r="U26" t="n">
+        <v>255</v>
+      </c>
+      <c r="V26" t="n">
+        <v>800</v>
+      </c>
+      <c r="W26" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X26" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC26" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF26" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (7).xlsx</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L27" t="n">
+        <v>4</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P27" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>135</v>
+      </c>
+      <c r="T27" t="n">
+        <v>36</v>
+      </c>
+      <c r="U27" t="n">
+        <v>255</v>
+      </c>
+      <c r="V27" t="n">
+        <v>800</v>
+      </c>
+      <c r="W27" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X27" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC27" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF27" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (8).xlsx</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L28" t="n">
+        <v>4</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P28" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>135</v>
+      </c>
+      <c r="T28" t="n">
+        <v>36</v>
+      </c>
+      <c r="U28" t="n">
+        <v>255</v>
+      </c>
+      <c r="V28" t="n">
+        <v>800</v>
+      </c>
+      <c r="W28" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X28" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC28" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF28" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본 (9).xlsx</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L29" t="n">
+        <v>4</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P29" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>135</v>
+      </c>
+      <c r="T29" t="n">
+        <v>36</v>
+      </c>
+      <c r="U29" t="n">
+        <v>255</v>
+      </c>
+      <c r="V29" t="n">
+        <v>800</v>
+      </c>
+      <c r="W29" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X29" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC29" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF29" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터 - 복사본.xlsx</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L30" t="n">
+        <v>4</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P30" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>135</v>
+      </c>
+      <c r="T30" t="n">
+        <v>36</v>
+      </c>
+      <c r="U30" t="n">
+        <v>255</v>
+      </c>
+      <c r="V30" t="n">
+        <v>800</v>
+      </c>
+      <c r="W30" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X30" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC30" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF30" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>23876098</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>5.북부여성발전센터.xlsx</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BEPA2022-01512123</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>test@test.or.kr</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>관리팀</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>김정락</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>02-3399-7604</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>eqroger@naver.com</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>서울시 북부여성발전센터</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>서울시 노원구 중계동 501-9</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>서울시 노원구 동일로207길 50</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L31" t="n">
+        <v>4</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>철근콘크리트</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>남</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P31" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>135</v>
+      </c>
+      <c r="T31" t="n">
+        <v>36</v>
+      </c>
+      <c r="U31" t="n">
+        <v>255</v>
+      </c>
+      <c r="V31" t="n">
+        <v>800</v>
+      </c>
+      <c r="W31" s="1" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="X31" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>예</t>
+        </is>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>810(별동층축 창업보육센터)</t>
+        </is>
+      </c>
+      <c r="AC31" t="n">
+        <v>2011</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t>교육연구시설</t>
+        </is>
+      </c>
+      <c r="AF31" t="n">
+        <v>24212016310</v>
+      </c>
+      <c r="AG31" t="n">
         <v>23876098</v>
       </c>
     </row>

</xml_diff>